<commit_message>
Print ALL result tables when running the script
add latest results to the excel
</commit_message>
<xml_diff>
--- a/price_pressure_results.xlsx
+++ b/price_pressure_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\git\GFSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFA33F0-C296-4303-AFD1-8CE072E11643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1336B266-8E02-4AE8-9E0A-EA89E4A52AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28E768B6-081E-48C5-BB84-B16AA56637EA}"/>
+    <workbookView xWindow="-21870" yWindow="4890" windowWidth="21600" windowHeight="15150" xr2:uid="{28E768B6-081E-48C5-BB84-B16AA56637EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Inclusions" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="24">
   <si>
     <t>Volumes</t>
   </si>
@@ -89,19 +89,34 @@
     <t>% &gt; 0</t>
   </si>
   <si>
-    <t>2021 \ 30 -&gt; 14</t>
-  </si>
-  <si>
     <t>Returns</t>
   </si>
   <si>
     <t>Exclusion Day</t>
+  </si>
+  <si>
+    <t>All \ 30 -&gt; 40</t>
+  </si>
+  <si>
+    <t>2021 \ 30 -&gt; 40</t>
+  </si>
+  <si>
+    <t>Volatility 5 days pre and post</t>
+  </si>
+  <si>
+    <t>Volatility 80 days</t>
+  </si>
+  <si>
+    <t>Volatility 80 day pre and post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -237,17 +252,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -260,10 +320,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,6 +341,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC46546D-798F-470E-B9D8-602ABC384CC1}">
-  <dimension ref="B2:W34"/>
+  <dimension ref="B2:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,155 +696,155 @@
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="22" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="24"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="22" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="24"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="25" t="s">
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="23" t="s">
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="24"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="T5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="7"/>
-      <c r="W5" s="8" t="s">
+      <c r="V5" s="6"/>
+      <c r="W5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -762,34 +852,34 @@
         <v>22</v>
       </c>
       <c r="D6" s="1">
-        <v>1.2431289999999999</v>
+        <v>1.644449</v>
       </c>
       <c r="E6" s="1">
-        <v>0.83943599999999996</v>
+        <v>0.88194700000000004</v>
       </c>
       <c r="F6" s="1">
-        <v>1.3585050000000001</v>
+        <v>3.4273389999999999</v>
       </c>
       <c r="G6" s="1">
-        <v>0.188719</v>
+        <v>2.5300000000000001E-3</v>
       </c>
       <c r="H6" s="3">
-        <v>50</v>
+        <v>81.818181999999993</v>
       </c>
       <c r="I6" s="1">
-        <v>1.338989</v>
+        <v>1.3191729999999999</v>
       </c>
       <c r="J6" s="1">
-        <v>1.0848869999999999</v>
+        <v>1.099871</v>
       </c>
       <c r="K6" s="1">
-        <v>3.277155</v>
+        <v>3.0435509999999999</v>
       </c>
       <c r="L6" s="1">
-        <v>1.407E-3</v>
+        <v>2.931E-3</v>
       </c>
       <c r="M6" s="3">
-        <v>55.454545000000003</v>
+        <v>51.818182</v>
       </c>
       <c r="N6" s="1">
         <v>1.4736130000000001</v>
@@ -822,7 +912,7 @@
         <v>41.818182</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
@@ -843,7 +933,7 @@
       <c r="U7" s="1"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -851,34 +941,34 @@
         <v>4</v>
       </c>
       <c r="D8" s="1">
-        <v>1.055982</v>
+        <v>1.0785899999999999</v>
       </c>
       <c r="E8" s="1">
-        <v>0.35248000000000002</v>
+        <v>0.25134400000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>0.31764500000000001</v>
+        <v>0.62535499999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>0.77157900000000001</v>
+        <v>0.57607799999999998</v>
       </c>
       <c r="H8" s="3">
         <v>50</v>
       </c>
       <c r="I8" s="1">
-        <v>0.93304600000000004</v>
+        <v>0.86557700000000004</v>
       </c>
       <c r="J8" s="1">
-        <v>0.33958100000000002</v>
+        <v>0.29235699999999998</v>
       </c>
       <c r="K8" s="1">
-        <v>-0.88175099999999995</v>
+        <v>-2.0562529999999999</v>
       </c>
       <c r="L8" s="1">
-        <v>0.38893100000000003</v>
+        <v>5.3758E-2</v>
       </c>
       <c r="M8" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="N8" s="1">
         <v>3.2607379999999999</v>
@@ -911,7 +1001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -919,34 +1009,34 @@
         <v>18</v>
       </c>
       <c r="D9" s="1">
-        <v>1.284718</v>
+        <v>1.770195</v>
       </c>
       <c r="E9" s="1">
-        <v>0.91567299999999996</v>
+        <v>0.92607700000000004</v>
       </c>
       <c r="F9" s="1">
-        <v>1.3191999999999999</v>
+        <v>3.5284970000000002</v>
       </c>
       <c r="G9" s="1">
-        <v>0.204596</v>
+        <v>2.5799999999999998E-3</v>
       </c>
       <c r="H9" s="3">
-        <v>50</v>
+        <v>88.888889000000006</v>
       </c>
       <c r="I9" s="1">
-        <v>1.429198</v>
+        <v>1.419972</v>
       </c>
       <c r="J9" s="1">
-        <v>1.1711499999999999</v>
+        <v>1.1860889999999999</v>
       </c>
       <c r="K9" s="1">
-        <v>3.4766949999999999</v>
+        <v>3.3591129999999998</v>
       </c>
       <c r="L9" s="1">
-        <v>7.8700000000000005E-4</v>
+        <v>1.1529999999999999E-3</v>
       </c>
       <c r="M9" s="3">
-        <v>58.888888999999999</v>
+        <v>56.666666999999997</v>
       </c>
       <c r="N9" s="1">
         <v>1.0764739999999999</v>
@@ -979,7 +1069,7 @@
         <v>35.555556000000003</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
@@ -1003,7 +1093,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>2021</v>
       </c>
@@ -1011,31 +1101,31 @@
         <v>12</v>
       </c>
       <c r="D11" s="1">
-        <v>1.033919</v>
+        <v>1.7749919999999999</v>
       </c>
       <c r="E11" s="1">
-        <v>0.53023500000000001</v>
+        <v>1.1109610000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>0.22159499999999999</v>
+        <v>2.4165130000000001</v>
       </c>
       <c r="G11" s="1">
-        <v>0.82869000000000004</v>
+        <v>3.4217999999999998E-2</v>
       </c>
       <c r="H11" s="3">
-        <v>33.333333000000003</v>
+        <v>83.333332999999996</v>
       </c>
       <c r="I11" s="1">
-        <v>1.307677</v>
+        <v>1.3446750000000001</v>
       </c>
       <c r="J11" s="1">
-        <v>0.99914599999999998</v>
+        <v>1.049925</v>
       </c>
       <c r="K11" s="1">
-        <v>2.3852910000000001</v>
+        <v>2.542888</v>
       </c>
       <c r="L11" s="1">
-        <v>2.0296000000000002E-2</v>
+        <v>1.3637E-2</v>
       </c>
       <c r="M11" s="3">
         <v>53.333333000000003</v>
@@ -1071,7 +1161,7 @@
         <v>31.666667</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
@@ -1093,286 +1183,358 @@
       <c r="U12" s="1"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="17">
         <v>10</v>
       </c>
-      <c r="D13" s="14">
-        <v>0.895783</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0.44518400000000002</v>
-      </c>
-      <c r="F13" s="14">
-        <v>-0.74028799999999995</v>
-      </c>
-      <c r="G13" s="14">
-        <v>0.47799199999999997</v>
+      <c r="D13" s="13">
+        <v>1.7850710000000001</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1.2204930000000001</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2.034106</v>
+      </c>
+      <c r="G13" s="13">
+        <v>7.2452000000000003E-2</v>
       </c>
       <c r="H13" s="3">
-        <v>20</v>
-      </c>
-      <c r="I13" s="14">
-        <v>1.1770370000000001</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0.663964</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1.8854070000000001</v>
-      </c>
-      <c r="L13" s="14">
-        <v>6.5310999999999994E-2</v>
+        <v>80</v>
+      </c>
+      <c r="I13" s="13">
+        <v>1.221435</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0.76002400000000003</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2.0601780000000001</v>
+      </c>
+      <c r="L13" s="13">
+        <v>4.4712000000000002E-2</v>
       </c>
       <c r="M13" s="3">
         <v>50</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="13">
         <v>0.86744299999999996</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="13">
         <v>0.16159299999999999</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="13">
         <v>-2.5940690000000002</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="13">
         <v>2.9019E-2</v>
       </c>
       <c r="R13" s="3">
         <v>20</v>
       </c>
-      <c r="S13" s="14">
+      <c r="S13" s="13">
         <v>0.88013399999999997</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="13">
         <v>0.23327800000000001</v>
       </c>
-      <c r="U13" s="14">
+      <c r="U13" s="13">
         <v>-3.6333639999999998</v>
       </c>
-      <c r="V13" s="14">
+      <c r="V13" s="13">
         <v>6.69E-4</v>
       </c>
       <c r="W13" s="3">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C14" s="15">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="26">
         <v>2</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="27">
         <v>1.7245980000000001</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="13">
         <v>0.40503400000000001</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="13">
         <v>2.5300020000000001</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="13">
         <v>0.23963000000000001</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="13">
         <v>100</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="27">
         <v>1.9608749999999999</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="13">
         <v>1.890846</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="13">
         <v>1.606981</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="13">
         <v>0.14252100000000001</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="3">
         <v>70</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="13">
         <v>1.1604650000000001</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="13">
         <v>0.45057599999999998</v>
       </c>
-      <c r="P14" s="9">
+      <c r="P14" s="13">
         <v>0.50364900000000001</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q14" s="13">
         <v>0.70297699999999996</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="3">
         <v>50</v>
       </c>
-      <c r="S14" s="9">
+      <c r="S14" s="13">
         <v>0.92485200000000001</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="13">
         <v>0.29874099999999998</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="13">
         <v>-0.79547199999999996</v>
       </c>
-      <c r="V14" s="9">
+      <c r="V14" s="13">
         <v>0.44680999999999998</v>
       </c>
-      <c r="W14" s="10">
+      <c r="W14" s="3">
         <v>40</v>
       </c>
     </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="28">
+        <v>12</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1.527263</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.48293399999999997</v>
+      </c>
+      <c r="F15" s="8">
+        <v>3.782073</v>
+      </c>
+      <c r="G15" s="8">
+        <v>3.0360000000000001E-3</v>
+      </c>
+      <c r="H15" s="8">
+        <v>83.333332999999996</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1.4006209999999999</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1.319215</v>
+      </c>
+      <c r="K15" s="8">
+        <v>2.352306</v>
+      </c>
+      <c r="L15" s="8">
+        <v>2.2013000000000001E-2</v>
+      </c>
+      <c r="M15" s="8">
+        <v>53.333333000000003</v>
+      </c>
+      <c r="N15" s="8">
+        <v>1.978755</v>
+      </c>
+      <c r="O15" s="8">
+        <v>2.3547210000000001</v>
+      </c>
+      <c r="P15" s="8">
+        <v>1.4398770000000001</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>0.17774899999999999</v>
+      </c>
+      <c r="R15" s="8">
+        <v>75</v>
+      </c>
+      <c r="S15" s="8">
+        <v>1.307639</v>
+      </c>
+      <c r="T15" s="8">
+        <v>1.195457</v>
+      </c>
+      <c r="U15" s="8">
+        <v>1.9933449999999999</v>
+      </c>
+      <c r="V15" s="8">
+        <v>5.0854000000000003E-2</v>
+      </c>
+      <c r="W15" s="8">
+        <v>51.666666999999997</v>
+      </c>
+      <c r="X15" s="26"/>
+    </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="24"/>
+      <c r="C22" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="23"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="22" t="s">
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="24"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="23"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="25" t="s">
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="25" t="s">
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="23" t="s">
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="24"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
+      <c r="V24" s="22"/>
+      <c r="W24" s="23"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="N25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O25" s="7" t="s">
+      <c r="O25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P25" s="7" t="s">
+      <c r="P25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q25" s="7" t="s">
+      <c r="Q25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R25" s="8" t="s">
+      <c r="R25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S25" s="7" t="s">
+      <c r="S25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="T25" s="7" t="s">
+      <c r="T25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U25" s="7" t="s">
+      <c r="U25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V25" s="7" t="s">
+      <c r="V25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W25" s="8" t="s">
+      <c r="W25" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1383,40 +1545,40 @@
       <c r="C26" s="2">
         <v>22</v>
       </c>
-      <c r="D26" s="11">
-        <v>9.2400000000000002E-4</v>
-      </c>
-      <c r="E26" s="11">
-        <v>1.8586999999999999E-2</v>
+      <c r="D26" s="10">
+        <v>1.536E-3</v>
+      </c>
+      <c r="E26" s="10">
+        <v>2.427E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>0.23325699999999999</v>
+        <v>0.29680400000000001</v>
       </c>
       <c r="G26" s="1">
-        <v>0.81781999999999999</v>
+        <v>0.76953199999999999</v>
       </c>
       <c r="H26" s="3">
-        <v>50</v>
-      </c>
-      <c r="I26" s="11">
-        <v>3.862E-3</v>
-      </c>
-      <c r="J26" s="11">
-        <v>2.0306000000000001E-2</v>
+        <v>40.909090999999997</v>
+      </c>
+      <c r="I26" s="10">
+        <v>-3.0400000000000002E-4</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1.9162999999999999E-2</v>
       </c>
       <c r="K26" s="1">
-        <v>1.994901</v>
+        <v>-0.166432</v>
       </c>
       <c r="L26" s="1">
-        <v>4.8549000000000002E-2</v>
+        <v>0.86812599999999995</v>
       </c>
       <c r="M26" s="3">
-        <v>56.363636</v>
-      </c>
-      <c r="N26" s="11">
+        <v>46.363636</v>
+      </c>
+      <c r="N26" s="10">
         <v>8.0759999999999998E-3</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="10">
         <v>2.2318999999999999E-2</v>
       </c>
       <c r="P26" s="1">
@@ -1428,10 +1590,10 @@
       <c r="R26" s="3">
         <v>72.727272999999997</v>
       </c>
-      <c r="S26" s="11">
+      <c r="S26" s="10">
         <v>-2.4740000000000001E-3</v>
       </c>
-      <c r="T26" s="11">
+      <c r="T26" s="10">
         <v>2.0730999999999999E-2</v>
       </c>
       <c r="U26" s="1">
@@ -1447,20 +1609,20 @@
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
       <c r="K27" s="1"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
       <c r="U27" s="1"/>
       <c r="W27" s="3"/>
     </row>
@@ -1471,40 +1633,40 @@
       <c r="C28" s="2">
         <v>4</v>
       </c>
-      <c r="D28" s="11">
-        <v>7.1299999999999998E-4</v>
-      </c>
-      <c r="E28" s="11">
-        <v>2.0274E-2</v>
+      <c r="D28" s="10">
+        <v>1.1868E-2</v>
+      </c>
+      <c r="E28" s="10">
+        <v>2.7518000000000001E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>7.0370000000000002E-2</v>
+        <v>0.86259200000000003</v>
       </c>
       <c r="G28" s="1">
-        <v>0.94832700000000003</v>
+        <v>0.45180300000000001</v>
       </c>
       <c r="H28" s="3">
-        <v>75</v>
-      </c>
-      <c r="I28" s="11">
-        <v>-2.7079999999999999E-3</v>
-      </c>
-      <c r="J28" s="11">
-        <v>2.4209999999999999E-2</v>
+        <v>50</v>
+      </c>
+      <c r="I28" s="10">
+        <v>6.8479999999999999E-3</v>
+      </c>
+      <c r="J28" s="10">
+        <v>1.9576E-2</v>
       </c>
       <c r="K28" s="1">
-        <v>-0.50026099999999996</v>
+        <v>1.5642990000000001</v>
       </c>
       <c r="L28" s="1">
-        <v>0.622637</v>
+        <v>0.13425100000000001</v>
       </c>
       <c r="M28" s="3">
-        <v>50</v>
-      </c>
-      <c r="N28" s="11">
+        <v>65</v>
+      </c>
+      <c r="N28" s="10">
         <v>-1.8270000000000002E-2</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="10">
         <v>2.4621000000000001E-2</v>
       </c>
       <c r="P28" s="1">
@@ -1516,10 +1678,10 @@
       <c r="R28" s="3">
         <v>25</v>
       </c>
-      <c r="S28" s="11">
+      <c r="S28" s="10">
         <v>-9.3089999999999996E-3</v>
       </c>
-      <c r="T28" s="11">
+      <c r="T28" s="10">
         <v>2.0558E-2</v>
       </c>
       <c r="U28" s="1">
@@ -1539,40 +1701,40 @@
       <c r="C29" s="2">
         <v>18</v>
       </c>
-      <c r="D29" s="11">
-        <v>9.7099999999999997E-4</v>
-      </c>
-      <c r="E29" s="11">
-        <v>1.8821000000000001E-2</v>
+      <c r="D29" s="10">
+        <v>-7.6000000000000004E-4</v>
+      </c>
+      <c r="E29" s="10">
+        <v>2.3734000000000002E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>0.21893899999999999</v>
+        <v>-0.135909</v>
       </c>
       <c r="G29" s="1">
-        <v>0.82930400000000004</v>
+        <v>0.89349000000000001</v>
       </c>
       <c r="H29" s="3">
-        <v>44.444443999999997</v>
-      </c>
-      <c r="I29" s="11">
-        <v>5.3229999999999996E-3</v>
-      </c>
-      <c r="J29" s="11">
-        <v>1.9184E-2</v>
+        <v>38.888888999999999</v>
+      </c>
+      <c r="I29" s="10">
+        <v>-1.8929999999999999E-3</v>
+      </c>
+      <c r="J29" s="10">
+        <v>1.8811000000000001E-2</v>
       </c>
       <c r="K29" s="1">
-        <v>2.632088</v>
+        <v>-0.95484400000000003</v>
       </c>
       <c r="L29" s="1">
-        <v>1.0003E-2</v>
+        <v>0.34224300000000002</v>
       </c>
       <c r="M29" s="3">
-        <v>57.777777999999998</v>
-      </c>
-      <c r="N29" s="11">
+        <v>42.222222000000002</v>
+      </c>
+      <c r="N29" s="10">
         <v>1.3931000000000001E-2</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="10">
         <v>1.7571E-2</v>
       </c>
       <c r="P29" s="1">
@@ -1584,10 +1746,10 @@
       <c r="R29" s="3">
         <v>83.333332999999996</v>
       </c>
-      <c r="S29" s="11">
+      <c r="S29" s="10">
         <v>-9.5500000000000001E-4</v>
       </c>
-      <c r="T29" s="11">
+      <c r="T29" s="10">
         <v>2.0573999999999999E-2</v>
       </c>
       <c r="U29" s="1">
@@ -1603,23 +1765,23 @@
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="3"/>
@@ -1631,40 +1793,40 @@
       <c r="C31" s="2">
         <v>12</v>
       </c>
-      <c r="D31" s="11">
-        <v>5.1580000000000003E-3</v>
-      </c>
-      <c r="E31" s="11">
-        <v>2.0077999999999999E-2</v>
+      <c r="D31" s="10">
+        <v>5.215E-3</v>
+      </c>
+      <c r="E31" s="10">
+        <v>2.6357999999999999E-2</v>
       </c>
       <c r="F31" s="1">
-        <v>0.88988199999999995</v>
+        <v>0.68537999999999999</v>
       </c>
       <c r="G31" s="1">
-        <v>0.39257500000000001</v>
+        <v>0.50729100000000005</v>
       </c>
       <c r="H31" s="3">
         <v>50</v>
       </c>
-      <c r="I31" s="11">
-        <v>8.1899999999999994E-3</v>
-      </c>
-      <c r="J31" s="11">
-        <v>2.1089E-2</v>
+      <c r="I31" s="10">
+        <v>6.3900000000000003E-4</v>
+      </c>
+      <c r="J31" s="10">
+        <v>1.8737E-2</v>
       </c>
       <c r="K31" s="1">
-        <v>3.0083169999999999</v>
+        <v>0.26426300000000003</v>
       </c>
       <c r="L31" s="1">
-        <v>3.8579999999999999E-3</v>
+        <v>0.79249800000000004</v>
       </c>
       <c r="M31" s="3">
-        <v>61.666666999999997</v>
-      </c>
-      <c r="N31" s="11">
+        <v>48.333333000000003</v>
+      </c>
+      <c r="N31" s="10">
         <v>1.1657000000000001E-2</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="10">
         <v>1.6712999999999999E-2</v>
       </c>
       <c r="P31" s="1">
@@ -1676,10 +1838,10 @@
       <c r="R31" s="3">
         <v>83.333332999999996</v>
       </c>
-      <c r="S31" s="11">
+      <c r="S31" s="10">
         <v>-1.686E-3</v>
       </c>
-      <c r="T31" s="11">
+      <c r="T31" s="10">
         <v>2.1389999999999999E-2</v>
       </c>
       <c r="U31" s="1">
@@ -1695,163 +1857,682 @@
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
       <c r="K32" s="1"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
       <c r="U32" s="1"/>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="17">
         <v>10</v>
       </c>
-      <c r="D33" s="16">
-        <v>8.8999999999999999E-3</v>
-      </c>
-      <c r="E33" s="13">
-        <v>1.9290000000000002E-2</v>
-      </c>
-      <c r="F33" s="14">
-        <v>1.4590369999999999</v>
-      </c>
-      <c r="G33" s="14">
-        <v>0.17855599999999999</v>
+      <c r="D33" s="15">
+        <v>8.9689999999999995E-3</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2.6981000000000002E-2</v>
+      </c>
+      <c r="F33" s="13">
+        <v>1.0511980000000001</v>
+      </c>
+      <c r="G33" s="13">
+        <v>0.32057200000000002</v>
       </c>
       <c r="H33" s="3">
         <v>60</v>
       </c>
-      <c r="I33" s="13">
-        <v>9.8329999999999997E-3</v>
-      </c>
-      <c r="J33" s="13">
-        <v>1.8922999999999999E-2</v>
-      </c>
-      <c r="K33" s="14">
-        <v>3.674363</v>
-      </c>
-      <c r="L33" s="14">
-        <v>5.9000000000000003E-4</v>
+      <c r="I33" s="12">
+        <v>7.7099999999999998E-4</v>
+      </c>
+      <c r="J33" s="12">
+        <v>1.6177E-2</v>
+      </c>
+      <c r="K33" s="13">
+        <v>0.33721200000000001</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0.73739699999999997</v>
       </c>
       <c r="M33" s="3">
-        <v>66</v>
-      </c>
-      <c r="N33" s="13">
+        <v>50</v>
+      </c>
+      <c r="N33" s="12">
         <v>1.2029E-2</v>
       </c>
-      <c r="O33" s="13">
+      <c r="O33" s="12">
         <v>1.8442E-2</v>
       </c>
-      <c r="P33" s="14">
+      <c r="P33" s="13">
         <v>2.0625830000000001</v>
       </c>
-      <c r="Q33" s="14">
+      <c r="Q33" s="13">
         <v>6.9190000000000002E-2</v>
       </c>
       <c r="R33" s="3">
         <v>80</v>
       </c>
-      <c r="S33" s="13">
+      <c r="S33" s="12">
         <v>-2.5070000000000001E-3</v>
       </c>
-      <c r="T33" s="13">
+      <c r="T33" s="12">
         <v>2.2744E-2</v>
       </c>
-      <c r="U33" s="14">
+      <c r="U33" s="13">
         <v>-0.77948300000000004</v>
       </c>
-      <c r="V33" s="14">
+      <c r="V33" s="13">
         <v>0.439444</v>
       </c>
       <c r="W33" s="3">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="18">
+        <v>20</v>
+      </c>
+      <c r="C34" s="30">
         <v>2</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="15">
         <v>-1.3554E-2</v>
       </c>
       <c r="E34" s="12">
         <v>1.5657000000000001E-2</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="13">
         <v>-1.2242660000000001</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="13">
         <v>0.43602800000000003</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="4">
         <v>0</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="15">
         <v>-2.1999999999999999E-5</v>
       </c>
       <c r="J34" s="12">
         <v>2.9600000000000001E-2</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="13">
         <v>-2.3379999999999998E-3</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="13">
         <v>0.99818499999999999</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34" s="4">
         <v>40</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="15">
         <v>9.7990000000000004E-3</v>
       </c>
       <c r="O34" s="12">
         <v>1.8550000000000001E-3</v>
       </c>
-      <c r="P34" s="9">
+      <c r="P34" s="13">
         <v>7.470046</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q34" s="13">
         <v>8.4719000000000003E-2</v>
       </c>
-      <c r="R34" s="6">
+      <c r="R34" s="4">
         <v>100</v>
       </c>
-      <c r="S34" s="17">
+      <c r="S34" s="15">
         <v>2.418E-3</v>
       </c>
       <c r="T34" s="12">
         <v>1.2673E-2</v>
       </c>
-      <c r="U34" s="9">
+      <c r="U34" s="13">
         <v>0.60331900000000005</v>
       </c>
-      <c r="V34" s="9">
+      <c r="V34" s="13">
         <v>0.561191</v>
       </c>
-      <c r="W34" s="5">
+      <c r="W34" s="2">
         <v>60</v>
       </c>
     </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="14">
+        <v>12</v>
+      </c>
+      <c r="D35" s="16">
+        <v>-4.6579999999999998E-3</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2.0902E-2</v>
+      </c>
+      <c r="F35" s="8">
+        <v>-0.77205699999999999</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.45634799999999998</v>
+      </c>
+      <c r="H35" s="8">
+        <v>25</v>
+      </c>
+      <c r="I35" s="11">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="J35" s="11">
+        <v>2.1430000000000001E-2</v>
+      </c>
+      <c r="K35" s="8">
+        <v>-0.43387599999999998</v>
+      </c>
+      <c r="L35" s="8">
+        <v>0.66596100000000003</v>
+      </c>
+      <c r="M35" s="8">
+        <v>43.333333000000003</v>
+      </c>
+      <c r="N35" s="11">
+        <v>4.7819999999999998E-3</v>
+      </c>
+      <c r="O35" s="11">
+        <v>2.5429E-2</v>
+      </c>
+      <c r="P35" s="8">
+        <v>0.65143399999999996</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>0.52814099999999997</v>
+      </c>
+      <c r="R35" s="8">
+        <v>66.666667000000004</v>
+      </c>
+      <c r="S35" s="11">
+        <v>-2.4459999999999998E-3</v>
+      </c>
+      <c r="T35" s="11">
+        <v>1.9088000000000001E-2</v>
+      </c>
+      <c r="U35" s="8">
+        <v>-0.99239200000000005</v>
+      </c>
+      <c r="V35" s="8">
+        <v>0.32505899999999999</v>
+      </c>
+      <c r="W35" s="8">
+        <v>48.333333000000003</v>
+      </c>
+      <c r="X35" s="26"/>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="C37" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="26"/>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B38" s="20"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35"/>
+      <c r="W38" s="36"/>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C39" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="17">
+        <v>22</v>
+      </c>
+      <c r="D40" s="39">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="E40" s="39">
+        <v>1.0628E-2</v>
+      </c>
+      <c r="F40" s="13">
+        <v>3.545E-3</v>
+      </c>
+      <c r="G40" s="13">
+        <v>0.99720500000000001</v>
+      </c>
+      <c r="H40" s="3">
+        <v>45.454545000000003</v>
+      </c>
+      <c r="I40" s="39">
+        <v>2.2100000000000001E-4</v>
+      </c>
+      <c r="J40" s="39">
+        <v>9.4319999999999994E-3</v>
+      </c>
+      <c r="K40" s="13">
+        <v>0.109792</v>
+      </c>
+      <c r="L40" s="13">
+        <v>0.91361700000000001</v>
+      </c>
+      <c r="M40" s="3">
+        <v>45.454545000000003</v>
+      </c>
+      <c r="N40" s="39">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="O40" s="39">
+        <v>5.8719999999999996E-3</v>
+      </c>
+      <c r="P40" s="13">
+        <v>1.277962</v>
+      </c>
+      <c r="Q40" s="13">
+        <v>0.21520900000000001</v>
+      </c>
+      <c r="R40" s="3">
+        <v>63.636364</v>
+      </c>
+      <c r="S40" s="39">
+        <v>1.4660000000000001E-3</v>
+      </c>
+      <c r="T40" s="39">
+        <v>5.5380000000000004E-3</v>
+      </c>
+      <c r="U40" s="13">
+        <v>1.2417020000000001</v>
+      </c>
+      <c r="V40" s="13">
+        <v>0.22803699999999999</v>
+      </c>
+      <c r="W40" s="3">
+        <v>59.090909000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C41" s="17"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="39"/>
+      <c r="T41" s="39"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="3"/>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="17">
+        <v>10</v>
+      </c>
+      <c r="D42" s="39">
+        <v>-5.2099999999999998E-4</v>
+      </c>
+      <c r="E42" s="39">
+        <v>6.3550000000000004E-3</v>
+      </c>
+      <c r="F42" s="13">
+        <v>-0.25941599999999998</v>
+      </c>
+      <c r="G42" s="13">
+        <v>0.80115000000000003</v>
+      </c>
+      <c r="H42" s="3">
+        <v>40</v>
+      </c>
+      <c r="I42" s="39">
+        <v>-1.085E-3</v>
+      </c>
+      <c r="J42" s="39">
+        <v>8.4279999999999997E-3</v>
+      </c>
+      <c r="K42" s="13">
+        <v>-0.40725699999999998</v>
+      </c>
+      <c r="L42" s="13">
+        <v>0.69333500000000003</v>
+      </c>
+      <c r="M42" s="3">
+        <v>40</v>
+      </c>
+      <c r="N42" s="39">
+        <v>5.4120000000000001E-3</v>
+      </c>
+      <c r="O42" s="39">
+        <v>4.0590000000000001E-3</v>
+      </c>
+      <c r="P42" s="13">
+        <v>4.2161689999999998</v>
+      </c>
+      <c r="Q42" s="13">
+        <v>2.2520000000000001E-3</v>
+      </c>
+      <c r="R42" s="3">
+        <v>100</v>
+      </c>
+      <c r="S42" s="39">
+        <v>5.0619999999999997E-3</v>
+      </c>
+      <c r="T42" s="39">
+        <v>3.5609999999999999E-3</v>
+      </c>
+      <c r="U42" s="13">
+        <v>4.4950349999999997</v>
+      </c>
+      <c r="V42" s="13">
+        <v>1.5E-3</v>
+      </c>
+      <c r="W42" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="17">
+        <v>2</v>
+      </c>
+      <c r="D43" s="39">
+        <v>1.3974E-2</v>
+      </c>
+      <c r="E43" s="39">
+        <v>3.4919999999999999E-3</v>
+      </c>
+      <c r="F43" s="13">
+        <v>5.6587069999999997</v>
+      </c>
+      <c r="G43" s="13">
+        <v>0.11135299999999999</v>
+      </c>
+      <c r="H43" s="3">
+        <v>100</v>
+      </c>
+      <c r="I43" s="39">
+        <v>-1.167E-2</v>
+      </c>
+      <c r="J43" s="39">
+        <v>1.2378999999999999E-2</v>
+      </c>
+      <c r="K43" s="13">
+        <v>-1.333218</v>
+      </c>
+      <c r="L43" s="13">
+        <v>0.409692</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="39">
+        <v>-9.9700000000000006E-4</v>
+      </c>
+      <c r="O43" s="39">
+        <v>3.64E-3</v>
+      </c>
+      <c r="P43" s="13">
+        <v>-0.38747500000000001</v>
+      </c>
+      <c r="Q43" s="13">
+        <v>0.76466599999999996</v>
+      </c>
+      <c r="R43" s="3">
+        <v>50</v>
+      </c>
+      <c r="S43" s="39">
+        <v>-7.9900000000000001E-4</v>
+      </c>
+      <c r="T43" s="39">
+        <v>1.402E-3</v>
+      </c>
+      <c r="U43" s="13">
+        <v>-0.80521100000000001</v>
+      </c>
+      <c r="V43" s="13">
+        <v>0.56842899999999996</v>
+      </c>
+      <c r="W43" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="19">
+        <v>12</v>
+      </c>
+      <c r="D44" s="40">
+        <v>4.4900000000000002E-4</v>
+      </c>
+      <c r="E44" s="40">
+        <v>1.3495999999999999E-2</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.11529</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.91029300000000002</v>
+      </c>
+      <c r="H44" s="9">
+        <v>50</v>
+      </c>
+      <c r="I44" s="40">
+        <v>1.3090000000000001E-3</v>
+      </c>
+      <c r="J44" s="40">
+        <v>1.0434000000000001E-2</v>
+      </c>
+      <c r="K44" s="8">
+        <v>0.43465599999999999</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.67221600000000004</v>
+      </c>
+      <c r="M44" s="9">
+        <v>50</v>
+      </c>
+      <c r="N44" s="40">
+        <v>-1.5770000000000001E-3</v>
+      </c>
+      <c r="O44" s="40">
+        <v>5.3030000000000004E-3</v>
+      </c>
+      <c r="P44" s="8">
+        <v>-1.0299450000000001</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>0.32514999999999999</v>
+      </c>
+      <c r="R44" s="9">
+        <v>33.333333000000003</v>
+      </c>
+      <c r="S44" s="40">
+        <v>-1.5299999999999999E-3</v>
+      </c>
+      <c r="T44" s="40">
+        <v>5.1599999999999997E-3</v>
+      </c>
+      <c r="U44" s="8">
+        <v>-1.027514</v>
+      </c>
+      <c r="V44" s="8">
+        <v>0.32624300000000001</v>
+      </c>
+      <c r="W44" s="9">
+        <v>33.333333000000003</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="S38:W38"/>
+    <mergeCell ref="N37:W37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="I38:M38"/>
+    <mergeCell ref="C37:M37"/>
+    <mergeCell ref="N38:R38"/>
     <mergeCell ref="C2:W2"/>
     <mergeCell ref="C22:W22"/>
     <mergeCell ref="C23:M23"/>
@@ -1874,10 +2555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97FBB80-8BF7-4CC7-82D4-2F3B8ABD25C2}">
-  <dimension ref="B2:W19"/>
+  <dimension ref="B2:W25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,152 +2569,152 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="24"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="24"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="25" t="s">
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="23" t="s">
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="24"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="O5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="P5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="T5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="V5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2198,217 +2879,217 @@
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="19">
         <v>8</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>1.580714</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>1.5549310000000001</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>1.056322</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>0.32590799999999998</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>50</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>1.4144410000000001</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>1.4426190000000001</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>1.8169420000000001</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <v>7.6916999999999999E-2</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <v>57.5</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="8">
         <v>0.71148900000000004</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="8">
         <v>0.20100299999999999</v>
       </c>
-      <c r="P9" s="9">
+      <c r="P9" s="8">
         <v>-4.0597989999999999</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="Q9" s="8">
         <v>4.8110000000000002E-3</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="9">
         <v>0</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="8">
         <v>0.68850699999999998</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="8">
         <v>0.27235999999999999</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="8">
         <v>-7.2332809999999998</v>
       </c>
-      <c r="V9" s="9">
+      <c r="V9" s="8">
         <v>1.027265E-8</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="9">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="22"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="22"/>
+      <c r="W12" s="23"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="24"/>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="24"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="23"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="25" t="s">
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="23" t="s">
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="24"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="23"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N15" s="7" t="s">
+      <c r="N15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="Q15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="S15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="T15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="U15" s="7" t="s">
+      <c r="U15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="V15" s="7" t="s">
+      <c r="V15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="W15" s="8" t="s">
+      <c r="W15" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2419,10 +3100,10 @@
       <c r="C16" s="2">
         <v>10</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>-6.8060000000000004E-3</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>4.5329000000000001E-2</v>
       </c>
       <c r="F16" s="1">
@@ -2434,10 +3115,10 @@
       <c r="H16" s="3">
         <v>40</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>-5.2769999999999996E-3</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <v>4.0162999999999997E-2</v>
       </c>
       <c r="K16" s="1">
@@ -2449,10 +3130,10 @@
       <c r="M16" s="3">
         <v>54</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <v>-1.2370000000000001E-2</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="10">
         <v>2.4551E-2</v>
       </c>
       <c r="P16" s="1">
@@ -2464,10 +3145,10 @@
       <c r="R16" s="3">
         <v>40</v>
       </c>
-      <c r="S16" s="11">
+      <c r="S16" s="10">
         <v>-1.7035000000000002E-2</v>
       </c>
-      <c r="T16" s="11">
+      <c r="T16" s="10">
         <v>5.3504999999999997E-2</v>
       </c>
       <c r="U16" s="1">
@@ -2483,20 +3164,20 @@
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="1"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
       <c r="U17" s="1"/>
       <c r="W17" s="3"/>
     </row>
@@ -2507,10 +3188,10 @@
       <c r="C18" s="2">
         <v>2</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>-2.3167E-2</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>1.6452000000000001E-2</v>
       </c>
       <c r="F18" s="1">
@@ -2522,10 +3203,10 @@
       <c r="H18" s="3">
         <v>0</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>1.8860000000000001E-3</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="10">
         <v>1.8408000000000001E-2</v>
       </c>
       <c r="K18" s="1">
@@ -2537,10 +3218,10 @@
       <c r="M18" s="3">
         <v>70</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>-1.1302E-2</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="10">
         <v>8.4220000000000007E-3</v>
       </c>
       <c r="P18" s="1">
@@ -2552,10 +3233,10 @@
       <c r="R18" s="3">
         <v>0</v>
       </c>
-      <c r="S18" s="11">
+      <c r="S18" s="10">
         <v>-1.5417E-2</v>
       </c>
-      <c r="T18" s="11">
+      <c r="T18" s="10">
         <v>2.0375000000000001E-2</v>
       </c>
       <c r="U18" s="1">
@@ -2572,72 +3253,290 @@
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="19">
         <v>8</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>-2.715E-3</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="11">
         <v>5.0075000000000001E-2</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>-0.153367</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0.882436</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="9">
         <v>50</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>-7.0670000000000004E-3</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>4.3955000000000001E-2</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="8">
         <v>-1.016883</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>0.31547599999999998</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>50</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="11">
         <v>-1.2638E-2</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="11">
         <v>2.7647999999999999E-2</v>
       </c>
-      <c r="P19" s="9">
+      <c r="P19" s="8">
         <v>-1.292834</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="Q19" s="8">
         <v>0.23710100000000001</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="9">
         <v>50</v>
       </c>
-      <c r="S19" s="12">
+      <c r="S19" s="11">
         <v>-1.7439E-2</v>
       </c>
-      <c r="T19" s="12">
+      <c r="T19" s="11">
         <v>5.9161999999999999E-2</v>
       </c>
-      <c r="U19" s="9">
+      <c r="U19" s="8">
         <v>-1.864309</v>
       </c>
-      <c r="V19" s="9">
+      <c r="V19" s="8">
         <v>6.9818000000000005E-2</v>
       </c>
-      <c r="W19" s="10">
+      <c r="W19" s="9">
         <v>47.5</v>
       </c>
     </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="33"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="20"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
+      <c r="V23" s="22"/>
+      <c r="W23" s="23"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C24" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="37">
+        <v>22</v>
+      </c>
+      <c r="D25" s="41">
+        <v>5.3600000000000002E-3</v>
+      </c>
+      <c r="E25" s="41">
+        <v>2.2537999999999999E-2</v>
+      </c>
+      <c r="F25" s="29">
+        <v>0.75203100000000001</v>
+      </c>
+      <c r="G25" s="29">
+        <v>0.47124100000000002</v>
+      </c>
+      <c r="H25" s="38">
+        <v>80</v>
+      </c>
+      <c r="I25" s="41">
+        <v>4.6369999999999996E-3</v>
+      </c>
+      <c r="J25" s="41">
+        <v>1.4120000000000001E-2</v>
+      </c>
+      <c r="K25" s="29">
+        <v>1.0385610000000001</v>
+      </c>
+      <c r="L25" s="29">
+        <v>0.32610499999999998</v>
+      </c>
+      <c r="M25" s="38">
+        <v>70</v>
+      </c>
+      <c r="N25" s="41">
+        <v>-1.5730999999999998E-2</v>
+      </c>
+      <c r="O25" s="41">
+        <v>4.9880000000000001E-2</v>
+      </c>
+      <c r="P25" s="29">
+        <v>-0.99729400000000001</v>
+      </c>
+      <c r="Q25" s="29">
+        <v>0.34467799999999998</v>
+      </c>
+      <c r="R25" s="38">
+        <v>50</v>
+      </c>
+      <c r="S25" s="41">
+        <v>-1.6917999999999999E-2</v>
+      </c>
+      <c r="T25" s="41">
+        <v>4.9225999999999999E-2</v>
+      </c>
+      <c r="U25" s="29">
+        <v>-1.086819</v>
+      </c>
+      <c r="V25" s="29">
+        <v>0.30536600000000003</v>
+      </c>
+      <c r="W25" s="38">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="20">
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="S23:W23"/>
+    <mergeCell ref="N22:W22"/>
+    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="I23:M23"/>
+    <mergeCell ref="C12:W12"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="N13:W13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="I14:M14"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="S14:W14"/>
     <mergeCell ref="C2:W2"/>
     <mergeCell ref="C3:M3"/>
     <mergeCell ref="N3:W3"/>
@@ -2645,13 +3544,6 @@
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="S4:W4"/>
-    <mergeCell ref="C12:W12"/>
-    <mergeCell ref="C13:M13"/>
-    <mergeCell ref="N13:W13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="S14:W14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>